<commit_message>
finished data_wrangle before final touches
</commit_message>
<xml_diff>
--- a/combined_df_fn_remove dups.xlsx
+++ b/combined_df_fn_remove dups.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lploughe/Documents/GitHub/iran_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2511ED7E-B7CD-DC40-874E-4FA8CBCCF3F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5298AD-63C8-B142-9692-0FFC227AF45E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23240" windowHeight="12700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$HG$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$HE$39</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="232">
   <si>
     <t>acantholimon_aspadanum</t>
   </si>
@@ -699,12 +699,6 @@
   </si>
   <si>
     <t>C4</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C5</t>
   </si>
   <si>
     <t>Th</t>
@@ -732,7 +726,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -740,19 +734,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -769,7 +764,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,15 +1080,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:HE39"/>
+  <dimension ref="A1:HC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="FB1" workbookViewId="0">
+      <selection activeCell="DO1" sqref="DO1:DO1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:213" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:211" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1307,434 +1302,428 @@
       <c r="BS1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>71</v>
       </c>
       <c r="BU1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BV1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BW1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BX1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BY1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="BZ1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="CA1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="CB1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="CC1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="CD1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="CE1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="CF1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="CG1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="CH1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="CI1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="CJ1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="CK1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="CL1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="CM1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="CN1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="CO1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="CP1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="CQ1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="CR1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="CS1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="CT1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="CU1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="CV1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="CW1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="CX1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="CY1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="CZ1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="DA1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="DB1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="DC1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="DD1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="DE1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="DF1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="DG1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="DH1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="DI1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="DJ1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="DK1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="DL1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="DM1" t="s">
-        <v>116</v>
-      </c>
-      <c r="DN1" t="s">
         <v>117</v>
       </c>
+      <c r="DN1" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="DO1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="DP1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="DQ1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="DR1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="DS1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="DT1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="DU1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="DV1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="DW1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="DX1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="DY1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="DZ1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="EA1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="EB1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="EC1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="ED1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="EE1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="EF1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="EG1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="EH1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="EI1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="EJ1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="EK1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="EL1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="EM1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="EN1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="EO1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="EP1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="EQ1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="ER1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="ES1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="ET1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="EU1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="EV1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="EW1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="EX1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="EY1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="EZ1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="FA1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="FB1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="FC1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="FD1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="FE1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="FF1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="FG1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="FH1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="FI1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="FJ1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="FK1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="FL1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="FM1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="FN1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="FO1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="FP1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="FQ1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="FR1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="FS1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="FT1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="FU1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="FV1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="FW1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="FX1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="FY1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="FZ1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="GA1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="GB1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="GC1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="GD1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="GE1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="GF1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="GG1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="GH1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="GI1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="GJ1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="GK1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="GL1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="GM1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="GN1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="GO1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="GP1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="GQ1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="GR1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="GS1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="GT1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="GU1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="GV1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="GW1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="GX1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="GY1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="GZ1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="HA1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="HB1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="HC1" t="s">
-        <v>210</v>
-      </c>
-      <c r="HD1" t="s">
-        <v>211</v>
-      </c>
-      <c r="HE1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:213" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:211" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>213</v>
       </c>
@@ -1948,62 +1937,62 @@
       <c r="BS2" t="s">
         <v>213</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BT2" s="1" t="s">
         <v>222</v>
       </c>
       <c r="BU2" t="s">
+        <v>213</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>213</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>213</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>213</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>213</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>221</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CL2" t="s">
         <v>222</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>213</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>213</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>213</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>213</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>221</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>213</v>
       </c>
       <c r="CM2" t="s">
         <v>222</v>
@@ -2015,328 +2004,328 @@
         <v>222</v>
       </c>
       <c r="CP2" t="s">
+        <v>221</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>213</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>221</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>221</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>221</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DN2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DQ2" t="s">
         <v>222</v>
       </c>
-      <c r="CQ2" t="s">
-        <v>221</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>221</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>221</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>221</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>221</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>221</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>213</v>
-      </c>
       <c r="DR2" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="DS2" t="s">
         <v>222</v>
       </c>
       <c r="DT2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>221</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>221</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>221</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>221</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>221</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EG2" t="s">
         <v>222</v>
       </c>
-      <c r="DU2" t="s">
+      <c r="EH2" t="s">
+        <v>221</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>221</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>213</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>213</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>221</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>221</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>213</v>
+      </c>
+      <c r="EZ2" t="s">
+        <v>221</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>221</v>
+      </c>
+      <c r="FB2" t="s">
+        <v>221</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>221</v>
+      </c>
+      <c r="FD2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FE2" t="s">
+        <v>221</v>
+      </c>
+      <c r="FF2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FG2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FH2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FI2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FJ2" t="s">
+        <v>221</v>
+      </c>
+      <c r="FK2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FL2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FM2" t="s">
         <v>222</v>
       </c>
-      <c r="DV2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>221</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>221</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>221</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>221</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>221</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EI2" t="s">
+      <c r="FN2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FP2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FQ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FT2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FW2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FX2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>213</v>
+      </c>
+      <c r="FZ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="GA2" t="s">
+        <v>213</v>
+      </c>
+      <c r="GB2" t="s">
+        <v>213</v>
+      </c>
+      <c r="GC2" t="s">
+        <v>213</v>
+      </c>
+      <c r="GD2" t="s">
+        <v>221</v>
+      </c>
+      <c r="GE2" t="s">
+        <v>221</v>
+      </c>
+      <c r="GF2" t="s">
+        <v>221</v>
+      </c>
+      <c r="GG2" t="s">
+        <v>221</v>
+      </c>
+      <c r="GH2" t="s">
+        <v>213</v>
+      </c>
+      <c r="GI2" t="s">
+        <v>213</v>
+      </c>
+      <c r="GJ2" t="s">
+        <v>213</v>
+      </c>
+      <c r="GK2" t="s">
+        <v>213</v>
+      </c>
+      <c r="GL2" t="s">
+        <v>213</v>
+      </c>
+      <c r="GM2" t="s">
+        <v>221</v>
+      </c>
+      <c r="GN2" t="s">
+        <v>221</v>
+      </c>
+      <c r="GO2" t="s">
+        <v>221</v>
+      </c>
+      <c r="GP2" t="s">
         <v>222</v>
       </c>
-      <c r="EJ2" t="s">
-        <v>221</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>221</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>213</v>
-      </c>
-      <c r="ES2" t="s">
-        <v>213</v>
-      </c>
-      <c r="ET2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EV2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EW2" t="s">
-        <v>221</v>
-      </c>
-      <c r="EX2" t="s">
-        <v>213</v>
-      </c>
-      <c r="EY2" t="s">
-        <v>221</v>
-      </c>
-      <c r="EZ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FA2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FB2" t="s">
-        <v>221</v>
-      </c>
-      <c r="FC2" t="s">
-        <v>221</v>
-      </c>
-      <c r="FD2" t="s">
-        <v>221</v>
-      </c>
-      <c r="FE2" t="s">
-        <v>221</v>
-      </c>
-      <c r="FF2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FG2" t="s">
-        <v>221</v>
-      </c>
-      <c r="FH2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FI2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FJ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FK2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FL2" t="s">
-        <v>221</v>
-      </c>
-      <c r="FM2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FN2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FO2" t="s">
+      <c r="GQ2" t="s">
         <v>222</v>
       </c>
-      <c r="FP2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FQ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FR2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FS2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FT2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FU2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FV2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FW2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FX2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FY2" t="s">
-        <v>213</v>
-      </c>
-      <c r="FZ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GA2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GB2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GC2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GD2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GE2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GF2" t="s">
-        <v>221</v>
-      </c>
-      <c r="GG2" t="s">
-        <v>221</v>
-      </c>
-      <c r="GH2" t="s">
-        <v>221</v>
-      </c>
-      <c r="GI2" t="s">
-        <v>221</v>
-      </c>
-      <c r="GJ2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GK2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GL2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GM2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GN2" t="s">
-        <v>213</v>
-      </c>
-      <c r="GO2" t="s">
-        <v>221</v>
-      </c>
-      <c r="GP2" t="s">
-        <v>221</v>
-      </c>
-      <c r="GQ2" t="s">
-        <v>221</v>
-      </c>
       <c r="GR2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="GS2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="GT2" t="s">
         <v>213</v>
@@ -2357,7 +2346,7 @@
         <v>213</v>
       </c>
       <c r="GZ2" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="HA2" t="s">
         <v>213</v>
@@ -2368,14 +2357,8 @@
       <c r="HC2" t="s">
         <v>213</v>
       </c>
-      <c r="HD2" t="s">
-        <v>221</v>
-      </c>
-      <c r="HE2" t="s">
-        <v>213</v>
-      </c>
     </row>
-    <row r="3" spans="1:213" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:211" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -2395,19 +2378,19 @@
         <v>217</v>
       </c>
       <c r="G3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J3" t="s">
         <v>220</v>
       </c>
       <c r="K3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L3" t="s">
         <v>217</v>
@@ -2464,7 +2447,7 @@
         <v>217</v>
       </c>
       <c r="AD3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AE3" t="s">
         <v>215</v>
@@ -2494,472 +2477,472 @@
         <v>215</v>
       </c>
       <c r="AN3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>228</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>229</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>225</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>225</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>225</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>225</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>225</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BT3" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>225</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>229</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CL3" t="s">
+        <v>228</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>228</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>228</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>228</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CV3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CY3" t="s">
+        <v>217</v>
+      </c>
+      <c r="CZ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DA3" t="s">
+        <v>225</v>
+      </c>
+      <c r="DB3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DC3" t="s">
+        <v>226</v>
+      </c>
+      <c r="DD3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DE3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DF3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DG3" t="s">
+        <v>225</v>
+      </c>
+      <c r="DH3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DI3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DJ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DK3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DL3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DM3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DN3" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="DO3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DP3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DQ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DR3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DS3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DT3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DU3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DV3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DW3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DX3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DY3" t="s">
+        <v>217</v>
+      </c>
+      <c r="DZ3" t="s">
+        <v>215</v>
+      </c>
+      <c r="EA3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EB3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EC3" t="s">
+        <v>217</v>
+      </c>
+      <c r="ED3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EE3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EF3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EG3" t="s">
+        <v>220</v>
+      </c>
+      <c r="EH3" t="s">
+        <v>228</v>
+      </c>
+      <c r="EI3" t="s">
+        <v>225</v>
+      </c>
+      <c r="EJ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EK3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EL3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EM3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EN3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EO3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EP3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EQ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="ER3" t="s">
+        <v>217</v>
+      </c>
+      <c r="ES3" t="s">
+        <v>217</v>
+      </c>
+      <c r="ET3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EU3" t="s">
+        <v>225</v>
+      </c>
+      <c r="EV3" t="s">
+        <v>230</v>
+      </c>
+      <c r="EW3" t="s">
+        <v>228</v>
+      </c>
+      <c r="EX3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EY3" t="s">
+        <v>217</v>
+      </c>
+      <c r="EZ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FA3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FB3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FC3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FD3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FE3" t="s">
         <v>227</v>
       </c>
-      <c r="AO3" t="s">
-        <v>227</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>227</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>227</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>217</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>230</v>
-      </c>
-      <c r="AW3" t="s">
+      <c r="FF3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FG3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FH3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FI3" t="s">
         <v>231</v>
       </c>
-      <c r="AX3" t="s">
-        <v>217</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>217</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>227</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>227</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>231</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>227</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>227</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>227</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>227</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BQ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BT3" t="s">
-        <v>230</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>230</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>227</v>
-      </c>
-      <c r="BW3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>217</v>
-      </c>
-      <c r="BZ3" t="s">
+      <c r="FJ3" t="s">
         <v>215</v>
       </c>
-      <c r="CA3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CB3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CF3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CG3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CJ3" t="s">
-        <v>231</v>
-      </c>
-      <c r="CK3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CL3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CM3" t="s">
-        <v>230</v>
-      </c>
-      <c r="CN3" t="s">
-        <v>230</v>
-      </c>
-      <c r="CO3" t="s">
-        <v>230</v>
-      </c>
-      <c r="CP3" t="s">
-        <v>230</v>
-      </c>
-      <c r="CQ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CR3" t="s">
-        <v>231</v>
-      </c>
-      <c r="CS3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CT3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CU3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CV3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CW3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CX3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CY3" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DA3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DB3" t="s">
-        <v>227</v>
-      </c>
-      <c r="DC3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DD3" t="s">
+      <c r="FK3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FL3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FM3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FN3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FO3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FP3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FQ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FR3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FS3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FT3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FU3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FV3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FW3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FX3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FY3" t="s">
+        <v>217</v>
+      </c>
+      <c r="FZ3" t="s">
+        <v>217</v>
+      </c>
+      <c r="GA3" t="s">
+        <v>217</v>
+      </c>
+      <c r="GB3" t="s">
+        <v>217</v>
+      </c>
+      <c r="GC3" t="s">
+        <v>217</v>
+      </c>
+      <c r="GD3" t="s">
         <v>228</v>
       </c>
-      <c r="DE3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DF3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DG3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DH3" t="s">
-        <v>227</v>
-      </c>
-      <c r="DI3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DJ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DK3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DL3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DM3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DN3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DO3" t="s">
-        <v>230</v>
-      </c>
-      <c r="DP3" t="s">
-        <v>220</v>
-      </c>
-      <c r="DQ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DR3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DS3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DT3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DU3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DV3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DW3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DX3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DY3" t="s">
-        <v>217</v>
-      </c>
-      <c r="DZ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EA3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EB3" t="s">
+      <c r="GE3" t="s">
+        <v>228</v>
+      </c>
+      <c r="GF3" t="s">
+        <v>217</v>
+      </c>
+      <c r="GG3" t="s">
+        <v>217</v>
+      </c>
+      <c r="GH3" t="s">
+        <v>217</v>
+      </c>
+      <c r="GI3" t="s">
+        <v>217</v>
+      </c>
+      <c r="GJ3" t="s">
         <v>215</v>
       </c>
-      <c r="EC3" t="s">
-        <v>217</v>
-      </c>
-      <c r="ED3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EE3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EF3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EG3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EH3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EI3" t="s">
-        <v>220</v>
-      </c>
-      <c r="EJ3" t="s">
-        <v>230</v>
-      </c>
-      <c r="EK3" t="s">
-        <v>227</v>
-      </c>
-      <c r="EL3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EM3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EN3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EO3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EP3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EQ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="ER3" t="s">
-        <v>217</v>
-      </c>
-      <c r="ES3" t="s">
-        <v>217</v>
-      </c>
-      <c r="ET3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EU3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EV3" t="s">
-        <v>217</v>
-      </c>
-      <c r="EW3" t="s">
-        <v>227</v>
-      </c>
-      <c r="EX3" t="s">
-        <v>232</v>
-      </c>
-      <c r="EY3" t="s">
-        <v>230</v>
-      </c>
-      <c r="EZ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FA3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FB3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FC3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FD3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FE3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FF3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FG3" t="s">
-        <v>229</v>
-      </c>
-      <c r="FH3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FI3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FJ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FK3" t="s">
-        <v>233</v>
-      </c>
-      <c r="FL3" t="s">
+      <c r="GK3" t="s">
         <v>215</v>
       </c>
-      <c r="FM3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FN3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FO3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FP3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FQ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FR3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FS3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FT3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FU3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FV3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FW3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FX3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FY3" t="s">
-        <v>217</v>
-      </c>
-      <c r="FZ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="GA3" t="s">
-        <v>217</v>
-      </c>
-      <c r="GB3" t="s">
-        <v>217</v>
-      </c>
-      <c r="GC3" t="s">
-        <v>217</v>
-      </c>
-      <c r="GD3" t="s">
-        <v>217</v>
-      </c>
-      <c r="GE3" t="s">
-        <v>217</v>
-      </c>
-      <c r="GF3" t="s">
-        <v>230</v>
-      </c>
-      <c r="GG3" t="s">
-        <v>230</v>
-      </c>
-      <c r="GH3" t="s">
-        <v>217</v>
-      </c>
-      <c r="GI3" t="s">
-        <v>217</v>
-      </c>
-      <c r="GJ3" t="s">
-        <v>217</v>
-      </c>
-      <c r="GK3" t="s">
-        <v>217</v>
-      </c>
       <c r="GL3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="GM3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="GN3" t="s">
         <v>217</v>
@@ -2977,13 +2960,13 @@
         <v>217</v>
       </c>
       <c r="GS3" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="GT3" t="s">
         <v>217</v>
       </c>
       <c r="GU3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="GV3" t="s">
         <v>217</v>
@@ -3009,14 +2992,8 @@
       <c r="HC3" t="s">
         <v>217</v>
       </c>
-      <c r="HD3" t="s">
-        <v>217</v>
-      </c>
-      <c r="HE3" t="s">
-        <v>217</v>
-      </c>
     </row>
-    <row r="4" spans="1:213" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:211" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>214</v>
       </c>
@@ -3033,7 +3010,7 @@
         <v>214</v>
       </c>
       <c r="F4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G4" t="s">
         <v>214</v>
@@ -3123,7 +3100,7 @@
         <v>218</v>
       </c>
       <c r="AJ4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="AK4" t="s">
         <v>218</v>
@@ -3153,7 +3130,7 @@
         <v>218</v>
       </c>
       <c r="AT4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="AU4" t="s">
         <v>218</v>
@@ -3186,7 +3163,7 @@
         <v>218</v>
       </c>
       <c r="BE4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="BF4" t="s">
         <v>218</v>
@@ -3198,7 +3175,7 @@
         <v>218</v>
       </c>
       <c r="BI4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="BJ4" t="s">
         <v>218</v>
@@ -3230,11 +3207,11 @@
       <c r="BS4" t="s">
         <v>218</v>
       </c>
-      <c r="BT4" t="s">
-        <v>218</v>
+      <c r="BT4" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="BU4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="BV4" t="s">
         <v>218</v>
@@ -3258,7 +3235,7 @@
         <v>218</v>
       </c>
       <c r="CC4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="CD4" t="s">
         <v>218</v>
@@ -3279,22 +3256,22 @@
         <v>218</v>
       </c>
       <c r="CJ4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="CK4" t="s">
         <v>218</v>
       </c>
       <c r="CL4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="CM4" t="s">
         <v>214</v>
       </c>
       <c r="CN4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="CO4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="CP4" t="s">
         <v>214</v>
@@ -3303,7 +3280,7 @@
         <v>214</v>
       </c>
       <c r="CR4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="CS4" t="s">
         <v>218</v>
@@ -3312,34 +3289,34 @@
         <v>218</v>
       </c>
       <c r="CU4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="CV4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="CW4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="CX4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="CY4" t="s">
         <v>218</v>
       </c>
       <c r="CZ4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="DA4" t="s">
         <v>214</v>
       </c>
       <c r="DB4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="DC4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="DD4" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="DE4" t="s">
         <v>218</v>
@@ -3366,10 +3343,10 @@
         <v>218</v>
       </c>
       <c r="DM4" t="s">
-        <v>218</v>
-      </c>
-      <c r="DN4" t="s">
-        <v>214</v>
+        <v>214</v>
+      </c>
+      <c r="DN4" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="DO4" t="s">
         <v>218</v>
@@ -3378,10 +3355,10 @@
         <v>218</v>
       </c>
       <c r="DQ4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="DR4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="DS4" t="s">
         <v>214</v>
@@ -3390,7 +3367,7 @@
         <v>214</v>
       </c>
       <c r="DU4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="DV4" t="s">
         <v>218</v>
@@ -3399,19 +3376,19 @@
         <v>218</v>
       </c>
       <c r="DX4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="DY4" t="s">
         <v>218</v>
       </c>
       <c r="DZ4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="EA4" t="s">
         <v>218</v>
       </c>
       <c r="EB4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="EC4" t="s">
         <v>218</v>
@@ -3423,7 +3400,7 @@
         <v>218</v>
       </c>
       <c r="EF4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="EG4" t="s">
         <v>218</v>
@@ -3444,7 +3421,7 @@
         <v>218</v>
       </c>
       <c r="EM4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="EN4" t="s">
         <v>218</v>
@@ -3453,10 +3430,10 @@
         <v>214</v>
       </c>
       <c r="EP4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="EQ4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="ER4" t="s">
         <v>214</v>
@@ -3471,7 +3448,7 @@
         <v>218</v>
       </c>
       <c r="EV4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="EW4" t="s">
         <v>218</v>
@@ -3483,13 +3460,13 @@
         <v>218</v>
       </c>
       <c r="EZ4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="FA4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="FB4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="FC4" t="s">
         <v>214</v>
@@ -3498,46 +3475,46 @@
         <v>218</v>
       </c>
       <c r="FE4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="FF4" t="s">
         <v>218</v>
       </c>
       <c r="FG4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="FH4" t="s">
         <v>218</v>
       </c>
       <c r="FI4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="FJ4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="FK4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="FL4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="FM4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="FN4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="FO4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="FP4" t="s">
         <v>214</v>
       </c>
       <c r="FQ4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="FR4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="FS4" t="s">
         <v>218</v>
@@ -3555,16 +3532,16 @@
         <v>218</v>
       </c>
       <c r="FX4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="FY4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="FZ4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="GA4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="GB4" t="s">
         <v>218</v>
@@ -3576,7 +3553,7 @@
         <v>218</v>
       </c>
       <c r="GE4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="GF4" t="s">
         <v>218</v>
@@ -3588,7 +3565,7 @@
         <v>218</v>
       </c>
       <c r="GI4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="GJ4" t="s">
         <v>218</v>
@@ -3600,22 +3577,22 @@
         <v>218</v>
       </c>
       <c r="GM4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="GN4" t="s">
         <v>218</v>
       </c>
       <c r="GO4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="GP4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="GQ4" t="s">
         <v>214</v>
       </c>
       <c r="GR4" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="GS4" t="s">
         <v>218</v>
@@ -3636,7 +3613,7 @@
         <v>218</v>
       </c>
       <c r="GY4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="GZ4" t="s">
         <v>218</v>
@@ -3648,16 +3625,10 @@
         <v>218</v>
       </c>
       <c r="HC4" t="s">
-        <v>214</v>
-      </c>
-      <c r="HD4" t="s">
-        <v>218</v>
-      </c>
-      <c r="HE4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:213" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:211" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -3674,7 +3645,7 @@
         <v>216</v>
       </c>
       <c r="F5" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="G5" t="s">
         <v>216</v>
@@ -3698,13 +3669,13 @@
         <v>216</v>
       </c>
       <c r="N5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O5" t="s">
         <v>216</v>
       </c>
       <c r="P5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="Q5" t="s">
         <v>216</v>
@@ -3713,7 +3684,7 @@
         <v>216</v>
       </c>
       <c r="S5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="T5" t="s">
         <v>216</v>
@@ -3740,7 +3711,7 @@
         <v>216</v>
       </c>
       <c r="AB5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AC5" t="s">
         <v>216</v>
@@ -3754,8 +3725,8 @@
       <c r="AF5" t="s">
         <v>219</v>
       </c>
-      <c r="AG5" s="1" t="s">
-        <v>225</v>
+      <c r="AG5" t="s">
+        <v>216</v>
       </c>
       <c r="AH5" t="s">
         <v>216</v>
@@ -3764,7 +3735,7 @@
         <v>216</v>
       </c>
       <c r="AJ5" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="AK5" t="s">
         <v>216</v>
@@ -3772,8 +3743,8 @@
       <c r="AL5" t="s">
         <v>216</v>
       </c>
-      <c r="AM5" s="1" t="s">
-        <v>226</v>
+      <c r="AM5" t="s">
+        <v>216</v>
       </c>
       <c r="AN5" t="s">
         <v>219</v>
@@ -3782,7 +3753,7 @@
         <v>216</v>
       </c>
       <c r="AP5" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="AQ5" t="s">
         <v>219</v>
@@ -3791,10 +3762,10 @@
         <v>219</v>
       </c>
       <c r="AS5" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="AT5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="AU5" t="s">
         <v>216</v>
@@ -3803,7 +3774,7 @@
         <v>216</v>
       </c>
       <c r="AW5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="AX5" t="s">
         <v>216</v>
@@ -3812,7 +3783,7 @@
         <v>216</v>
       </c>
       <c r="AZ5" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="BA5" t="s">
         <v>219</v>
@@ -3827,7 +3798,7 @@
         <v>216</v>
       </c>
       <c r="BE5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="BF5" t="s">
         <v>216</v>
@@ -3839,7 +3810,7 @@
         <v>216</v>
       </c>
       <c r="BI5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="BJ5" t="s">
         <v>216</v>
@@ -3871,8 +3842,8 @@
       <c r="BS5" t="s">
         <v>216</v>
       </c>
-      <c r="BT5" t="s">
-        <v>214</v>
+      <c r="BT5" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="BU5" t="s">
         <v>216</v>
@@ -3881,7 +3852,7 @@
         <v>216</v>
       </c>
       <c r="BW5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="BX5" t="s">
         <v>216</v>
@@ -3902,7 +3873,7 @@
         <v>216</v>
       </c>
       <c r="CD5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="CE5" t="s">
         <v>216</v>
@@ -3920,7 +3891,7 @@
         <v>216</v>
       </c>
       <c r="CJ5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="CK5" t="s">
         <v>216</v>
@@ -3932,10 +3903,10 @@
         <v>216</v>
       </c>
       <c r="CN5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="CO5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="CP5" t="s">
         <v>216</v>
@@ -3944,7 +3915,7 @@
         <v>216</v>
       </c>
       <c r="CR5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="CS5" t="s">
         <v>216</v>
@@ -3956,286 +3927,286 @@
         <v>216</v>
       </c>
       <c r="CV5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="CW5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="CX5" t="s">
+        <v>216</v>
+      </c>
+      <c r="CY5" t="s">
+        <v>216</v>
+      </c>
+      <c r="CZ5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DA5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DB5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DC5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DD5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DE5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DF5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DG5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DH5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DI5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DJ5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DK5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DL5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DM5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DN5" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="DO5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DP5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DQ5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DR5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DS5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DT5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DU5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DV5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DW5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DX5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DY5" t="s">
+        <v>216</v>
+      </c>
+      <c r="DZ5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EA5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EB5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EC5" t="s">
+        <v>216</v>
+      </c>
+      <c r="ED5" t="s">
+        <v>224</v>
+      </c>
+      <c r="EE5" t="s">
         <v>219</v>
-      </c>
-      <c r="CY5" t="s">
-        <v>214</v>
-      </c>
-      <c r="CZ5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DA5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DB5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DC5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DD5" t="s">
-        <v>218</v>
-      </c>
-      <c r="DE5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DF5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DG5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DH5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DI5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DJ5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DK5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DL5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DM5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DN5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DO5" t="s">
-        <v>214</v>
-      </c>
-      <c r="DP5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DQ5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DR5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DS5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DT5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DU5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DV5" t="s">
-        <v>214</v>
-      </c>
-      <c r="DW5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DX5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DY5" t="s">
-        <v>216</v>
-      </c>
-      <c r="DZ5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EA5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EB5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EC5" t="s">
-        <v>216</v>
-      </c>
-      <c r="ED5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EE5" t="s">
-        <v>216</v>
       </c>
       <c r="EF5" t="s">
         <v>224</v>
       </c>
       <c r="EG5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EH5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EI5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EJ5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EK5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EL5" t="s">
         <v>219</v>
       </c>
-      <c r="EH5" t="s">
+      <c r="EM5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EN5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EO5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EP5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EQ5" t="s">
+        <v>216</v>
+      </c>
+      <c r="ER5" t="s">
+        <v>216</v>
+      </c>
+      <c r="ES5" t="s">
+        <v>216</v>
+      </c>
+      <c r="ET5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EU5" t="s">
         <v>224</v>
       </c>
-      <c r="EI5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EJ5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EK5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EL5" t="s">
-        <v>214</v>
-      </c>
-      <c r="EM5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EN5" t="s">
-        <v>214</v>
-      </c>
-      <c r="EO5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EP5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EQ5" t="s">
-        <v>216</v>
-      </c>
-      <c r="ER5" t="s">
-        <v>216</v>
-      </c>
-      <c r="ES5" t="s">
-        <v>216</v>
-      </c>
-      <c r="ET5" t="s">
-        <v>216</v>
-      </c>
-      <c r="EU5" t="s">
-        <v>214</v>
-      </c>
       <c r="EV5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="EW5" t="s">
+        <v>219</v>
+      </c>
+      <c r="EX5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EY5" t="s">
+        <v>216</v>
+      </c>
+      <c r="EZ5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FA5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FB5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FC5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FD5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FE5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FF5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FG5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FH5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FI5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FJ5" t="s">
+        <v>219</v>
+      </c>
+      <c r="FK5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FL5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FM5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FN5" t="s">
         <v>224</v>
       </c>
-      <c r="EX5" t="s">
+      <c r="FO5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FP5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FQ5" t="s">
         <v>219</v>
       </c>
-      <c r="EY5" t="s">
-        <v>214</v>
-      </c>
-      <c r="EZ5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FA5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FB5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FC5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FD5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FE5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FF5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FG5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FH5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FI5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FJ5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FK5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FL5" t="s">
+      <c r="FR5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FS5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FT5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FU5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FV5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FW5" t="s">
+        <v>224</v>
+      </c>
+      <c r="FX5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FY5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FZ5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GA5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GB5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GC5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GD5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GE5" t="s">
         <v>219</v>
       </c>
-      <c r="FM5" t="s">
-        <v>214</v>
-      </c>
-      <c r="FN5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FO5" t="s">
-        <v>214</v>
-      </c>
-      <c r="FP5" t="s">
-        <v>224</v>
-      </c>
-      <c r="FQ5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FR5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FS5" t="s">
+      <c r="GF5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GG5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GH5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GI5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GJ5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GK5" t="s">
         <v>219</v>
-      </c>
-      <c r="FT5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FU5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FV5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FW5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FX5" t="s">
-        <v>216</v>
-      </c>
-      <c r="FY5" t="s">
-        <v>215</v>
-      </c>
-      <c r="FZ5" t="s">
-        <v>214</v>
-      </c>
-      <c r="GA5" t="s">
-        <v>214</v>
-      </c>
-      <c r="GB5" t="s">
-        <v>214</v>
-      </c>
-      <c r="GC5" t="s">
-        <v>216</v>
-      </c>
-      <c r="GD5" t="s">
-        <v>216</v>
-      </c>
-      <c r="GE5" t="s">
-        <v>216</v>
-      </c>
-      <c r="GF5" t="s">
-        <v>216</v>
-      </c>
-      <c r="GG5" t="s">
-        <v>219</v>
-      </c>
-      <c r="GH5" t="s">
-        <v>214</v>
-      </c>
-      <c r="GI5" t="s">
-        <v>216</v>
-      </c>
-      <c r="GJ5" t="s">
-        <v>216</v>
-      </c>
-      <c r="GK5" t="s">
-        <v>216</v>
       </c>
       <c r="GL5" t="s">
         <v>216</v>
@@ -4244,28 +4215,28 @@
         <v>219</v>
       </c>
       <c r="GN5" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="GO5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GP5" t="s">
         <v>219</v>
       </c>
-      <c r="GP5" t="s">
-        <v>224</v>
-      </c>
       <c r="GQ5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="GR5" t="s">
+        <v>216</v>
+      </c>
+      <c r="GS5" t="s">
         <v>219</v>
       </c>
-      <c r="GS5" t="s">
-        <v>214</v>
-      </c>
       <c r="GT5" t="s">
         <v>216</v>
       </c>
       <c r="GU5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="GV5" t="s">
         <v>216</v>
@@ -4289,187 +4260,6 @@
         <v>216</v>
       </c>
       <c r="HC5" t="s">
-        <v>216</v>
-      </c>
-      <c r="HD5" t="s">
-        <v>216</v>
-      </c>
-      <c r="HE5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="6" spans="1:213" x14ac:dyDescent="0.2">
-      <c r="F6" t="s">
-        <v>219</v>
-      </c>
-      <c r="N6" t="s">
-        <v>216</v>
-      </c>
-      <c r="P6" t="s">
-        <v>216</v>
-      </c>
-      <c r="S6" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>224</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>219</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>219</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>219</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>216</v>
-      </c>
-      <c r="BE6" t="s">
-        <v>216</v>
-      </c>
-      <c r="BI6" t="s">
-        <v>216</v>
-      </c>
-      <c r="BT6" t="s">
-        <v>216</v>
-      </c>
-      <c r="BW6" t="s">
-        <v>216</v>
-      </c>
-      <c r="CD6" t="s">
-        <v>216</v>
-      </c>
-      <c r="CJ6" t="s">
-        <v>216</v>
-      </c>
-      <c r="CN6" t="s">
-        <v>216</v>
-      </c>
-      <c r="CO6" t="s">
-        <v>216</v>
-      </c>
-      <c r="CR6" t="s">
-        <v>214</v>
-      </c>
-      <c r="CV6" t="s">
-        <v>224</v>
-      </c>
-      <c r="CY6" t="s">
-        <v>216</v>
-      </c>
-      <c r="DD6" t="s">
-        <v>214</v>
-      </c>
-      <c r="DO6" t="s">
-        <v>224</v>
-      </c>
-      <c r="DV6" t="s">
-        <v>216</v>
-      </c>
-      <c r="EL6" t="s">
-        <v>216</v>
-      </c>
-      <c r="EN6" t="s">
-        <v>219</v>
-      </c>
-      <c r="EU6" t="s">
-        <v>216</v>
-      </c>
-      <c r="EX6" t="s">
-        <v>216</v>
-      </c>
-      <c r="EY6" t="s">
-        <v>219</v>
-      </c>
-      <c r="FM6" t="s">
-        <v>219</v>
-      </c>
-      <c r="FO6" t="s">
-        <v>216</v>
-      </c>
-      <c r="FY6" t="s">
-        <v>224</v>
-      </c>
-      <c r="FZ6" t="s">
-        <v>216</v>
-      </c>
-      <c r="GA6" t="s">
-        <v>219</v>
-      </c>
-      <c r="GB6" t="s">
-        <v>216</v>
-      </c>
-      <c r="GH6" t="s">
-        <v>216</v>
-      </c>
-      <c r="GM6" t="s">
-        <v>216</v>
-      </c>
-      <c r="GS6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="7" spans="1:213" x14ac:dyDescent="0.2">
-      <c r="F7" t="s">
-        <v>216</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>216</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>216</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>216</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>216</v>
-      </c>
-      <c r="CR7" t="s">
-        <v>216</v>
-      </c>
-      <c r="CV7" t="s">
-        <v>216</v>
-      </c>
-      <c r="DD7" t="s">
-        <v>216</v>
-      </c>
-      <c r="DO7" t="s">
-        <v>216</v>
-      </c>
-      <c r="EN7" t="s">
-        <v>216</v>
-      </c>
-      <c r="EY7" t="s">
-        <v>216</v>
-      </c>
-      <c r="FM7" t="s">
-        <v>216</v>
-      </c>
-      <c r="FY7" t="s">
-        <v>216</v>
-      </c>
-      <c r="GA7" t="s">
-        <v>216</v>
-      </c>
-      <c r="GS7" t="s">
         <v>216</v>
       </c>
     </row>
@@ -4483,8 +4273,8 @@
     <row r="38" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="39" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="GL2:GM34">
-    <sortCondition descending="1" ref="GM1:GM39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="GJ2:GK34">
+    <sortCondition descending="1" ref="GK1:GK39"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4498,7 +4288,7 @@
       <selection sqref="A1:HE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:213" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>